<commit_message>
fixed data population issue and updated the grant upload excel sheet
</commit_message>
<xml_diff>
--- a/data/InOrderUploadTests/4grantUpload.xlsx
+++ b/data/InOrderUploadTests/4grantUpload.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\takoda\Documents\CS-Grad-Tracking\data\InOrderUploadTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonjunjin/CS-Grad-Tracking/data/InOrderUploadTests/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5887277B-8FC0-7B41-A634-6297B7558CF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15915" windowHeight="9900"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15920" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -32,16 +33,28 @@
     <t>Grant for testing</t>
   </si>
   <si>
-    <t>GRANT 2 for testing</t>
-  </si>
-  <si>
-    <t>dummy header</t>
+    <t>pi_type</t>
+  </si>
+  <si>
+    <t>cs_pi_name</t>
+  </si>
+  <si>
+    <t>other_pi_name</t>
+  </si>
+  <si>
+    <t>OTHER_PI</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>othertest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,34 +365,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>